<commit_message>
added deit loss and accuracy to excel
</commit_message>
<xml_diff>
--- a/loss_acc_for_graphs.xlsx
+++ b/loss_acc_for_graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthahay/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiran\Documents\Fall21\DeepLearningSeminar\coding-assignment-week-8-vit-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C4C8C3F-FCAE-5A4D-805E-0C2DB56273F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5795045F-89B4-4F79-97BB-7FAEBD177F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="1560" windowWidth="28040" windowHeight="16000" xr2:uid="{ABD42D1D-A641-FB40-A47F-DF2F71A33C85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABD42D1D-A641-FB40-A47F-DF2F71A33C85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>ViT</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>CIFAR-10</t>
+  </si>
+  <si>
+    <t>DeiT</t>
   </si>
 </sst>
 </file>
@@ -411,18 +414,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B87570-E25C-B94D-AE26-DA955205743B}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,12 +490,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -557,7 +560,7 @@
         <v>1.002</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -622,12 +625,12 @@
         <v>53.462499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -692,7 +695,7 @@
         <v>0.109</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -757,12 +760,12 @@
         <v>18.59375</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -827,7 +830,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -890,6 +893,416 @@
       </c>
       <c r="U12">
         <v>78.849999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2.38142881267949</v>
+      </c>
+      <c r="C16">
+        <v>2.3402747919684899</v>
+      </c>
+      <c r="D16">
+        <v>2.0297876063146001</v>
+      </c>
+      <c r="E16">
+        <v>1.5991922303249899</v>
+      </c>
+      <c r="F16">
+        <v>1.4425443912807201</v>
+      </c>
+      <c r="G16">
+        <v>1.36741580147492</v>
+      </c>
+      <c r="H16">
+        <v>1.2814129779213299</v>
+      </c>
+      <c r="I16">
+        <v>1.3011209149109599</v>
+      </c>
+      <c r="J16">
+        <v>1.3564058244228301</v>
+      </c>
+      <c r="K16">
+        <v>1.2828656105618701</v>
+      </c>
+      <c r="L16">
+        <v>1.2718531881508</v>
+      </c>
+      <c r="M16">
+        <v>1.2773549619473901</v>
+      </c>
+      <c r="N16">
+        <v>1.1894847154617301</v>
+      </c>
+      <c r="O16">
+        <v>1.2151779124611299</v>
+      </c>
+      <c r="P16">
+        <v>1.24914535252671</v>
+      </c>
+      <c r="Q16">
+        <v>1.2079322557700301</v>
+      </c>
+      <c r="R16">
+        <v>1.21191795248734</v>
+      </c>
+      <c r="S16">
+        <v>1.19468530228263</v>
+      </c>
+      <c r="T16">
+        <v>1.1078823381348599</v>
+      </c>
+      <c r="U16">
+        <v>1.20008581249337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>12.0625002365112</v>
+      </c>
+      <c r="C17">
+        <v>14.7625003967285</v>
+      </c>
+      <c r="D17">
+        <v>76.387503173828094</v>
+      </c>
+      <c r="E17">
+        <v>89.412502990722601</v>
+      </c>
+      <c r="F17">
+        <v>92.600002441406204</v>
+      </c>
+      <c r="G17">
+        <v>94.437502746581998</v>
+      </c>
+      <c r="H17">
+        <v>94.175002380371097</v>
+      </c>
+      <c r="I17">
+        <v>94.137502441406198</v>
+      </c>
+      <c r="J17">
+        <v>95.012501953124996</v>
+      </c>
+      <c r="K17">
+        <v>95.350002624511703</v>
+      </c>
+      <c r="L17">
+        <v>95.162502807617102</v>
+      </c>
+      <c r="M17">
+        <v>95.825002746582001</v>
+      </c>
+      <c r="N17">
+        <v>95.687502197265601</v>
+      </c>
+      <c r="O17">
+        <v>95.725002746582007</v>
+      </c>
+      <c r="P17">
+        <v>95.762502624511697</v>
+      </c>
+      <c r="Q17">
+        <v>95.812502197265601</v>
+      </c>
+      <c r="R17">
+        <v>95.950002319335894</v>
+      </c>
+      <c r="S17">
+        <v>96.112502197265599</v>
+      </c>
+      <c r="T17">
+        <v>96.162502380371095</v>
+      </c>
+      <c r="U17">
+        <v>96.162502075195306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>4.7773776572683504</v>
+      </c>
+      <c r="C20">
+        <v>4.7209026398866003</v>
+      </c>
+      <c r="D20">
+        <v>4.3020073382750796</v>
+      </c>
+      <c r="E20">
+        <v>3.6252780530763702</v>
+      </c>
+      <c r="F20">
+        <v>3.1442557832469098</v>
+      </c>
+      <c r="G20">
+        <v>2.7128629269807201</v>
+      </c>
+      <c r="H20">
+        <v>2.3086596260899999</v>
+      </c>
+      <c r="I20">
+        <v>2.148361750271</v>
+      </c>
+      <c r="J20">
+        <v>1.96025768570278</v>
+      </c>
+      <c r="K20">
+        <v>1.9582724182502</v>
+      </c>
+      <c r="L20">
+        <v>1.7233908746553499</v>
+      </c>
+      <c r="M20">
+        <v>1.74969106912612</v>
+      </c>
+      <c r="N20">
+        <v>1.64456712422163</v>
+      </c>
+      <c r="O20">
+        <v>1.57949196514876</v>
+      </c>
+      <c r="P20">
+        <v>1.58193930853968</v>
+      </c>
+      <c r="Q20">
+        <v>1.5167814778244999</v>
+      </c>
+      <c r="R20">
+        <v>1.5042027740374799</v>
+      </c>
+      <c r="S20">
+        <v>1.4967302990996301</v>
+      </c>
+      <c r="T20">
+        <v>1.4715914739214799</v>
+      </c>
+      <c r="U20">
+        <v>1.43566106842911</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>0.61443934984470805</v>
+      </c>
+      <c r="C21">
+        <v>0.61443934984470805</v>
+      </c>
+      <c r="D21">
+        <v>27.726574875792</v>
+      </c>
+      <c r="E21">
+        <v>44.162827838950399</v>
+      </c>
+      <c r="F21">
+        <v>64.746545800415603</v>
+      </c>
+      <c r="G21">
+        <v>69.508449958766107</v>
+      </c>
+      <c r="H21">
+        <v>76.958528263777595</v>
+      </c>
+      <c r="I21">
+        <v>78.955455024121505</v>
+      </c>
+      <c r="J21">
+        <v>78.571430821572505</v>
+      </c>
+      <c r="K21">
+        <v>79.953919300835196</v>
+      </c>
+      <c r="L21">
+        <v>80.952384913571905</v>
+      </c>
+      <c r="M21">
+        <v>83.486945789530495</v>
+      </c>
+      <c r="N21">
+        <v>83.640557706630702</v>
+      </c>
+      <c r="O21">
+        <v>82.872507051388794</v>
+      </c>
+      <c r="P21">
+        <v>84.024579448084594</v>
+      </c>
+      <c r="Q21">
+        <v>84.254994405579396</v>
+      </c>
+      <c r="R21">
+        <v>84.024580116096104</v>
+      </c>
+      <c r="S21">
+        <v>83.717361204085805</v>
+      </c>
+      <c r="T21">
+        <v>84.792630314277602</v>
+      </c>
+      <c r="U21">
+        <v>84.331798360094993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>2.2708631918980502</v>
+      </c>
+      <c r="C24">
+        <v>2.10866297422311</v>
+      </c>
+      <c r="D24">
+        <v>1.69960997807673</v>
+      </c>
+      <c r="E24">
+        <v>1.5880840501724101</v>
+      </c>
+      <c r="F24">
+        <v>1.52696154316266</v>
+      </c>
+      <c r="G24">
+        <v>1.5243850996860999</v>
+      </c>
+      <c r="H24">
+        <v>1.5362521422214901</v>
+      </c>
+      <c r="I24">
+        <v>1.46570869668936</v>
+      </c>
+      <c r="J24">
+        <v>1.4676731491700099</v>
+      </c>
+      <c r="K24">
+        <v>1.46148274005987</v>
+      </c>
+      <c r="L24">
+        <v>1.42804607550303</v>
+      </c>
+      <c r="M24">
+        <v>1.4317569870215101</v>
+      </c>
+      <c r="N24">
+        <v>1.40641588828502</v>
+      </c>
+      <c r="O24">
+        <v>1.40195413292982</v>
+      </c>
+      <c r="P24">
+        <v>1.3760134472296699</v>
+      </c>
+      <c r="Q24">
+        <v>1.3802266029211101</v>
+      </c>
+      <c r="R24">
+        <v>1.3791513161781499</v>
+      </c>
+      <c r="S24">
+        <v>1.3245098438018399</v>
+      </c>
+      <c r="T24">
+        <v>1.3455636903261501</v>
+      </c>
+      <c r="U24">
+        <v>1.32338791153369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>36.550001074218699</v>
+      </c>
+      <c r="C25">
+        <v>50.830001293945301</v>
+      </c>
+      <c r="D25">
+        <v>91.220002490234293</v>
+      </c>
+      <c r="E25">
+        <v>93.160002783203097</v>
+      </c>
+      <c r="F25">
+        <v>93.9600025878906</v>
+      </c>
+      <c r="G25">
+        <v>93.0200026855468</v>
+      </c>
+      <c r="H25">
+        <v>93.440002392578094</v>
+      </c>
+      <c r="I25">
+        <v>94.270002343749994</v>
+      </c>
+      <c r="J25">
+        <v>94.640002246093701</v>
+      </c>
+      <c r="K25">
+        <v>94.540002343750004</v>
+      </c>
+      <c r="L25">
+        <v>95.750002685546804</v>
+      </c>
+      <c r="M25">
+        <v>95.640002587890606</v>
+      </c>
+      <c r="N25">
+        <v>95.980002197265605</v>
+      </c>
+      <c r="O25">
+        <v>96.290002539062499</v>
+      </c>
+      <c r="P25">
+        <v>96.350001953125002</v>
+      </c>
+      <c r="Q25">
+        <v>96.440002685546801</v>
+      </c>
+      <c r="R25">
+        <v>96.670002929687499</v>
+      </c>
+      <c r="S25">
+        <v>96.650002685546795</v>
+      </c>
+      <c r="T25">
+        <v>96.620002832031204</v>
+      </c>
+      <c r="U25">
+        <v>96.900002294921805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>